<commit_message>
Local search fails to stay inside constraints. Adding Global Search options
</commit_message>
<xml_diff>
--- a/SystemParameters.xlsx
+++ b/SystemParameters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Python Projects\Optimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BD597CA1-541D-4CB6-B3CE-F91B9FB1272B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCCE036-41D1-4A9F-8C3C-DA4968B7F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24075" yWindow="720" windowWidth="24165" windowHeight="13590"/>
+    <workbookView xWindow="-28920" yWindow="-510" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
   <si>
     <t>Model</t>
   </si>
@@ -170,12 +170,15 @@
   </si>
   <si>
     <t>RZM_350_8</t>
+  </si>
+  <si>
+    <t>NLamps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -602,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,9 +626,10 @@
     <col min="10" max="10" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -662,8 +666,11 @@
       <c r="L1" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -701,8 +708,11 @@
       <c r="L2" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -740,8 +750,11 @@
       <c r="L3" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -779,8 +792,11 @@
       <c r="L4" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -818,8 +834,11 @@
       <c r="L5" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -857,8 +876,11 @@
       <c r="L6" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -896,8 +918,11 @@
       <c r="L7" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -935,8 +960,11 @@
       <c r="L8" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -974,8 +1002,11 @@
       <c r="L9" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1013,8 +1044,11 @@
       <c r="L10" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1052,8 +1086,11 @@
       <c r="L11" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1091,8 +1128,11 @@
       <c r="L12" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1130,8 +1170,11 @@
       <c r="L13" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1169,8 +1212,11 @@
       <c r="L14" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
@@ -1208,8 +1254,11 @@
       <c r="L15" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1247,8 +1296,11 @@
       <c r="L16" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1286,8 +1338,11 @@
       <c r="L17" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -1325,8 +1380,11 @@
       <c r="L18" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
@@ -1364,8 +1422,11 @@
       <c r="L19" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1403,8 +1464,11 @@
       <c r="L20" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
@@ -1442,8 +1506,11 @@
       <c r="L21" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -1481,8 +1548,11 @@
       <c r="L22" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -1520,8 +1590,11 @@
       <c r="L23" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
@@ -1559,8 +1632,11 @@
       <c r="L24" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
@@ -1598,8 +1674,11 @@
       <c r="L25" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1637,8 +1716,11 @@
       <c r="L26" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1676,8 +1758,11 @@
       <c r="L27" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1715,8 +1800,11 @@
       <c r="L28" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
@@ -1754,8 +1842,11 @@
       <c r="L29" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>11</v>
       </c>
@@ -1793,8 +1884,11 @@
       <c r="L30" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
@@ -1832,8 +1926,11 @@
       <c r="L31" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
@@ -1871,8 +1968,11 @@
       <c r="L32" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
@@ -1910,8 +2010,11 @@
       <c r="L33" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>22</v>
       </c>
@@ -1949,8 +2052,11 @@
       <c r="L34" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>22</v>
       </c>
@@ -1988,8 +2094,11 @@
       <c r="L35" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>12</v>
       </c>
@@ -2027,8 +2136,11 @@
       <c r="L36" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>12</v>
       </c>
@@ -2066,8 +2178,11 @@
       <c r="L37" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
@@ -2104,6 +2219,9 @@
       </c>
       <c r="L38" s="4">
         <v>100</v>
+      </c>
+      <c r="M38" s="8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready v1.07 Added features for the table. Added Pressure Drop
</commit_message>
<xml_diff>
--- a/SystemParameters.xlsx
+++ b/SystemParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Python Projects\Optimizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerts\Documents\Projects\Python\Optimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF683DEE-A372-4972-BE07-C00D663E67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45430313-E3D3-4664-A43D-37F364ADBC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1140" windowWidth="24165" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -160,19 +158,19 @@
     <t>NLamps</t>
   </si>
   <si>
-    <t>RZ-163HP</t>
-  </si>
-  <si>
-    <t>RZ-163UHP</t>
-  </si>
-  <si>
-    <t>RZ-163LP</t>
-  </si>
-  <si>
     <t>RZM-350_Marine</t>
   </si>
   <si>
     <t>RZM-350_Land</t>
+  </si>
+  <si>
+    <t>RZ-163_HP</t>
+  </si>
+  <si>
+    <t>RZ-163_UHP</t>
+  </si>
+  <si>
+    <t>RZ-163_Regular</t>
   </si>
 </sst>
 </file>
@@ -608,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +922,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2">
         <v>11</v>
@@ -934,7 +932,7 @@
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163LP-11</v>
+        <v>RZ-163_Regular-11</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -966,7 +964,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>12</v>
@@ -976,7 +974,7 @@
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163LP-12</v>
+        <v>RZ-163_Regular-12</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1008,7 +1006,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
         <v>13</v>
@@ -1018,7 +1016,7 @@
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163LP-13</v>
+        <v>RZ-163_Regular-13</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1050,7 +1048,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2">
         <v>14</v>
@@ -1060,7 +1058,7 @@
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163LP-14</v>
+        <v>RZ-163_Regular-14</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1092,7 +1090,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -1102,7 +1100,7 @@
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163HP-11</v>
+        <v>RZ-163_HP-11</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1134,7 +1132,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -1144,7 +1142,7 @@
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163HP-12</v>
+        <v>RZ-163_HP-12</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
@@ -1176,7 +1174,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -1186,7 +1184,7 @@
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163HP-13</v>
+        <v>RZ-163_HP-13</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -1218,7 +1216,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -1228,7 +1226,7 @@
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163HP-14</v>
+        <v>RZ-163_HP-14</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -1260,7 +1258,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2">
         <v>11</v>
@@ -1270,7 +1268,7 @@
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163UHP-11</v>
+        <v>RZ-163_UHP-11</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -1302,7 +1300,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2">
         <v>12</v>
@@ -1312,7 +1310,7 @@
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163UHP-12</v>
+        <v>RZ-163_UHP-12</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -1344,7 +1342,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2">
         <v>13</v>
@@ -1354,7 +1352,7 @@
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163UHP-13</v>
+        <v>RZ-163_UHP-13</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -1386,7 +1384,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2">
         <v>14</v>
@@ -1396,7 +1394,7 @@
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163UHP-14</v>
+        <v>RZ-163_UHP-14</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
@@ -1848,7 +1846,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" s="8">
         <v>8</v>
@@ -1890,7 +1888,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B31" s="8">
         <v>5</v>
@@ -2016,7 +2014,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B34" s="8">
         <v>8</v>
@@ -2058,7 +2056,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B35" s="8">
         <v>5</v>

</xml_diff>

<commit_message>
Ready v1.08 Dropped R-200 system. Fixed no-wrap for the entire calculator
</commit_message>
<xml_diff>
--- a/SystemParameters.xlsx
+++ b/SystemParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerts\Documents\Projects\Python\Optimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45430313-E3D3-4664-A43D-37F364ADBC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46891741-7367-446F-B2D0-4A51DB082724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="915" windowWidth="26280" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>DL</t>
-  </si>
-  <si>
     <t>RS-104</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>RZM-200</t>
   </si>
   <si>
-    <t>R-200</t>
-  </si>
-  <si>
     <t>Qmin vertical [m^3/h]</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>VF RED</t>
   </si>
   <si>
-    <t>R200_SDL</t>
-  </si>
-  <si>
     <t>CalcModule</t>
   </si>
   <si>
@@ -170,7 +158,7 @@
     <t>RZ-163_UHP</t>
   </si>
   <si>
-    <t>RZ-163_Regular</t>
+    <t>RZ-163_Reg</t>
   </si>
 </sst>
 </file>
@@ -604,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,81 +617,81 @@
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="str">
-        <f>_xlfn.CONCAT(A2,"-",B2)</f>
-        <v>R-200-SL</v>
+        <f t="shared" ref="D2:D36" si="0">_xlfn.CONCAT(A2,"-",B2)</f>
+        <v>RS-104-11</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="G2" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
-        <v>500</v>
-      </c>
-      <c r="I2" s="2">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2">
-        <v>99</v>
-      </c>
-      <c r="K2" s="2">
-        <v>25</v>
-      </c>
-      <c r="L2" s="2">
+        <v>140</v>
+      </c>
+      <c r="I2" s="3">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3">
+        <v>99</v>
+      </c>
+      <c r="K2" s="3">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3">
         <v>100</v>
       </c>
       <c r="M2" s="4">
@@ -712,38 +700,38 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D38" si="0">_xlfn.CONCAT(A3,"-",B3)</f>
-        <v>R-200-DL</v>
+        <f t="shared" si="0"/>
+        <v>RS-104-12</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="G3" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
-        <v>500</v>
-      </c>
-      <c r="I3" s="2">
+        <v>140</v>
+      </c>
+      <c r="I3" s="3">
         <v>25</v>
       </c>
       <c r="J3" s="3">
         <v>99</v>
       </c>
       <c r="K3" s="2">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L3" s="3">
         <v>100</v>
@@ -754,17 +742,17 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RS-104-11</v>
+        <v>RZ-104-11</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
@@ -784,7 +772,7 @@
       <c r="J4" s="3">
         <v>99</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>40</v>
       </c>
       <c r="L4" s="3">
@@ -796,17 +784,17 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RS-104-12</v>
+        <v>RZ-104-12</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -838,29 +826,29 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2">
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-104-11</v>
+        <v>RZ-163_Reg-11</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H6" s="2">
-        <v>140</v>
+        <v>360</v>
       </c>
       <c r="I6" s="3">
         <v>25</v>
@@ -880,29 +868,29 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-104-12</v>
+        <v>RZ-163_Reg-12</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2">
-        <v>140</v>
+        <v>360</v>
       </c>
       <c r="I7" s="3">
         <v>25</v>
@@ -922,17 +910,17 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_Regular-11</v>
+        <v>RZ-163_Reg-13</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -940,11 +928,11 @@
       <c r="F8" s="3">
         <v>6</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>30</v>
       </c>
-      <c r="H8" s="2">
-        <v>360</v>
+      <c r="H8" s="4">
+        <v>300</v>
       </c>
       <c r="I8" s="3">
         <v>25</v>
@@ -959,22 +947,22 @@
         <v>100</v>
       </c>
       <c r="M8" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_Regular-12</v>
+        <v>RZ-163_Reg-14</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -982,11 +970,11 @@
       <c r="F9" s="3">
         <v>6</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>30</v>
       </c>
-      <c r="H9" s="2">
-        <v>360</v>
+      <c r="H9" s="4">
+        <v>300</v>
       </c>
       <c r="I9" s="3">
         <v>25</v>
@@ -1001,22 +989,22 @@
         <v>100</v>
       </c>
       <c r="M9" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_Regular-13</v>
+        <v>RZ-163_HP-11</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1027,8 +1015,8 @@
       <c r="G10" s="3">
         <v>30</v>
       </c>
-      <c r="H10" s="4">
-        <v>300</v>
+      <c r="H10" s="3">
+        <v>360</v>
       </c>
       <c r="I10" s="3">
         <v>25</v>
@@ -1036,29 +1024,29 @@
       <c r="J10" s="3">
         <v>99</v>
       </c>
-      <c r="K10" s="2">
-        <v>40</v>
+      <c r="K10" s="3">
+        <v>25</v>
       </c>
       <c r="L10" s="3">
         <v>100</v>
       </c>
       <c r="M10" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_Regular-14</v>
+        <v>RZ-163_HP-12</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1069,8 +1057,8 @@
       <c r="G11" s="3">
         <v>30</v>
       </c>
-      <c r="H11" s="4">
-        <v>300</v>
+      <c r="H11" s="3">
+        <v>360</v>
       </c>
       <c r="I11" s="3">
         <v>25</v>
@@ -1078,29 +1066,29 @@
       <c r="J11" s="3">
         <v>99</v>
       </c>
-      <c r="K11" s="2">
-        <v>40</v>
+      <c r="K11" s="3">
+        <v>25</v>
       </c>
       <c r="L11" s="3">
         <v>100</v>
       </c>
       <c r="M11" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_HP-11</v>
+        <v>RZ-163_HP-13</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1112,7 +1100,7 @@
         <v>30</v>
       </c>
       <c r="H12" s="3">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="I12" s="3">
         <v>25</v>
@@ -1127,22 +1115,22 @@
         <v>100</v>
       </c>
       <c r="M12" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_HP-12</v>
+        <v>RZ-163_HP-14</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
@@ -1154,7 +1142,7 @@
         <v>30</v>
       </c>
       <c r="H13" s="3">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="I13" s="3">
         <v>25</v>
@@ -1169,22 +1157,22 @@
         <v>100</v>
       </c>
       <c r="M13" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_HP-13</v>
+        <v>RZ-163_UHP-11</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -1196,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="H14" s="3">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="I14" s="3">
         <v>25</v>
@@ -1211,22 +1199,22 @@
         <v>100</v>
       </c>
       <c r="M14" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_HP-14</v>
+        <v>RZ-163_UHP-12</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -1238,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="H15" s="3">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="I15" s="3">
         <v>25</v>
@@ -1253,22 +1241,22 @@
         <v>100</v>
       </c>
       <c r="M15" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_UHP-11</v>
+        <v>RZ-163_UHP-13</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -1279,8 +1267,8 @@
       <c r="G16" s="3">
         <v>30</v>
       </c>
-      <c r="H16" s="3">
-        <v>360</v>
+      <c r="H16" s="4">
+        <v>300</v>
       </c>
       <c r="I16" s="3">
         <v>25</v>
@@ -1295,22 +1283,22 @@
         <v>100</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-163_UHP-12</v>
+        <v>RZ-163_UHP-14</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -1321,8 +1309,8 @@
       <c r="G17" s="3">
         <v>30</v>
       </c>
-      <c r="H17" s="3">
-        <v>360</v>
+      <c r="H17" s="4">
+        <v>300</v>
       </c>
       <c r="I17" s="3">
         <v>25</v>
@@ -1337,40 +1325,40 @@
         <v>100</v>
       </c>
       <c r="M17" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>RZ-300-11</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <v>30</v>
       </c>
-      <c r="D18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>RZ-163_UHP-13</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3">
-        <v>30</v>
-      </c>
-      <c r="H18" s="4">
-        <v>300</v>
+      <c r="G18" s="2">
+        <v>150</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2200</v>
       </c>
       <c r="I18" s="3">
         <v>25</v>
       </c>
       <c r="J18" s="3">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K18" s="3">
         <v>25</v>
@@ -1379,40 +1367,40 @@
         <v>100</v>
       </c>
       <c r="M18" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B19" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>RZ-300-12</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
         <v>30</v>
       </c>
-      <c r="D19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>RZ-163_UHP-14</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>6</v>
-      </c>
       <c r="G19" s="3">
-        <v>30</v>
-      </c>
-      <c r="H19" s="4">
-        <v>300</v>
+        <v>150</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2200</v>
       </c>
       <c r="I19" s="3">
         <v>25</v>
       </c>
       <c r="J19" s="3">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K19" s="3">
         <v>25</v>
@@ -1421,22 +1409,22 @@
         <v>100</v>
       </c>
       <c r="M19" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-300-11</v>
+        <v>RZ-300-13</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1444,7 +1432,7 @@
       <c r="F20" s="3">
         <v>30</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>150</v>
       </c>
       <c r="H20" s="2">
@@ -1463,22 +1451,22 @@
         <v>100</v>
       </c>
       <c r="M20" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="B21" s="4">
+        <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-300-12</v>
+        <v>RZ-300-14</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1505,40 +1493,40 @@
         <v>100</v>
       </c>
       <c r="M21" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="2">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="4">
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-300-13</v>
+        <v>RZB-300-11</v>
       </c>
       <c r="E22" s="4">
         <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="G22" s="3">
         <v>150</v>
       </c>
       <c r="H22" s="2">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="I22" s="3">
         <v>25</v>
       </c>
       <c r="J22" s="3">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K22" s="3">
         <v>25</v>
@@ -1547,40 +1535,40 @@
         <v>100</v>
       </c>
       <c r="M22" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZ-300-14</v>
+        <v>RZB-300-12</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="G23" s="3">
         <v>150</v>
       </c>
       <c r="H23" s="2">
-        <v>2200</v>
+        <v>900</v>
       </c>
       <c r="I23" s="3">
         <v>25</v>
       </c>
       <c r="J23" s="3">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K23" s="3">
         <v>25</v>
@@ -1594,17 +1582,17 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZB-300-11</v>
+        <v>RZB-300-13</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
@@ -1616,7 +1604,7 @@
         <v>150</v>
       </c>
       <c r="H24" s="2">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="I24" s="3">
         <v>25</v>
@@ -1631,22 +1619,22 @@
         <v>100</v>
       </c>
       <c r="M24" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZB-300-12</v>
+        <v>RZB-300-14</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
@@ -1658,7 +1646,7 @@
         <v>150</v>
       </c>
       <c r="H25" s="2">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="I25" s="3">
         <v>25</v>
@@ -1673,34 +1661,34 @@
         <v>100</v>
       </c>
       <c r="M25" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZB-300-13</v>
+        <v>EP-600-2</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>150</v>
-      </c>
-      <c r="G26" s="3">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="G26" s="2">
+        <v>500</v>
       </c>
       <c r="H26" s="2">
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="I26" s="3">
         <v>25</v>
@@ -1715,34 +1703,34 @@
         <v>100</v>
       </c>
       <c r="M26" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZB-300-14</v>
+        <v>EP-600-4</v>
       </c>
       <c r="E27" s="4">
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>150</v>
-      </c>
-      <c r="G27" s="3">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="G27" s="2">
+        <v>500</v>
       </c>
       <c r="H27" s="2">
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="I27" s="3">
         <v>25</v>
@@ -1757,22 +1745,22 @@
         <v>100</v>
       </c>
       <c r="M27" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="4">
-        <v>2</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B28" s="8">
+        <v>8</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>EP-600-2</v>
+        <v>RZM-350_Land-8</v>
       </c>
       <c r="E28" s="4">
         <v>1</v>
@@ -1780,11 +1768,11 @@
       <c r="F28" s="3">
         <v>100</v>
       </c>
-      <c r="G28" s="2">
-        <v>500</v>
+      <c r="G28" s="3">
+        <v>100</v>
       </c>
       <c r="H28" s="2">
-        <v>3500</v>
+        <v>1150</v>
       </c>
       <c r="I28" s="3">
         <v>25</v>
@@ -1798,23 +1786,23 @@
       <c r="L28" s="3">
         <v>100</v>
       </c>
-      <c r="M28" s="4">
-        <v>2</v>
+      <c r="M28" s="8">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4">
-        <v>4</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B29" s="8">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>EP-600-4</v>
+        <v>RZM-350_Land-5</v>
       </c>
       <c r="E29" s="4">
         <v>1</v>
@@ -1822,11 +1810,11 @@
       <c r="F29" s="3">
         <v>100</v>
       </c>
-      <c r="G29" s="2">
-        <v>500</v>
+      <c r="G29" s="3">
+        <v>100</v>
       </c>
       <c r="H29" s="2">
-        <v>3500</v>
+        <v>1150</v>
       </c>
       <c r="I29" s="3">
         <v>25</v>
@@ -1840,203 +1828,203 @@
       <c r="L29" s="3">
         <v>100</v>
       </c>
-      <c r="M29" s="4">
-        <v>4</v>
+      <c r="M29" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B30" s="8">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZM-350_Land-8</v>
+        <v>RZMW-350-11</v>
       </c>
       <c r="E30" s="4">
         <v>1</v>
       </c>
-      <c r="F30" s="3">
-        <v>100</v>
-      </c>
-      <c r="G30" s="3">
-        <v>100</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="F30" s="4">
+        <v>100</v>
+      </c>
+      <c r="G30" s="4">
+        <v>100</v>
+      </c>
+      <c r="H30" s="4">
         <v>1150</v>
       </c>
-      <c r="I30" s="3">
-        <v>25</v>
-      </c>
-      <c r="J30" s="3">
-        <v>99</v>
-      </c>
-      <c r="K30" s="3">
-        <v>25</v>
-      </c>
-      <c r="L30" s="3">
+      <c r="I30" s="4">
+        <v>25</v>
+      </c>
+      <c r="J30" s="4">
+        <v>99</v>
+      </c>
+      <c r="K30" s="4">
+        <v>25</v>
+      </c>
+      <c r="L30" s="4">
         <v>100</v>
       </c>
       <c r="M30" s="8">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B31" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZM-350_Land-5</v>
+        <v>RZMW-350-7</v>
       </c>
       <c r="E31" s="4">
         <v>1</v>
       </c>
-      <c r="F31" s="3">
-        <v>100</v>
-      </c>
-      <c r="G31" s="3">
-        <v>100</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="F31" s="4">
+        <v>100</v>
+      </c>
+      <c r="G31" s="4">
+        <v>100</v>
+      </c>
+      <c r="H31" s="4">
         <v>1150</v>
       </c>
-      <c r="I31" s="3">
-        <v>25</v>
-      </c>
-      <c r="J31" s="3">
-        <v>99</v>
-      </c>
-      <c r="K31" s="3">
-        <v>25</v>
-      </c>
-      <c r="L31" s="3">
+      <c r="I31" s="4">
+        <v>25</v>
+      </c>
+      <c r="J31" s="4">
+        <v>99</v>
+      </c>
+      <c r="K31" s="4">
+        <v>25</v>
+      </c>
+      <c r="L31" s="4">
         <v>100</v>
       </c>
       <c r="M31" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B32" s="8">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZMW-350-11</v>
+        <v>RZM-350_Marine-8</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
       </c>
-      <c r="F32" s="4">
-        <v>100</v>
-      </c>
-      <c r="G32" s="4">
-        <v>100</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="F32" s="3">
+        <v>100</v>
+      </c>
+      <c r="G32" s="3">
+        <v>100</v>
+      </c>
+      <c r="H32" s="2">
         <v>1150</v>
       </c>
-      <c r="I32" s="4">
-        <v>25</v>
-      </c>
-      <c r="J32" s="4">
-        <v>99</v>
-      </c>
-      <c r="K32" s="4">
-        <v>25</v>
-      </c>
-      <c r="L32" s="4">
+      <c r="I32" s="3">
+        <v>25</v>
+      </c>
+      <c r="J32" s="3">
+        <v>99</v>
+      </c>
+      <c r="K32" s="3">
+        <v>25</v>
+      </c>
+      <c r="L32" s="3">
         <v>100</v>
       </c>
       <c r="M32" s="8">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B33" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZMW-350-7</v>
+        <v>RZM-350_Marine-5</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
       </c>
-      <c r="F33" s="4">
-        <v>100</v>
-      </c>
-      <c r="G33" s="4">
-        <v>100</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="F33" s="3">
+        <v>100</v>
+      </c>
+      <c r="G33" s="3">
+        <v>100</v>
+      </c>
+      <c r="H33" s="2">
         <v>1150</v>
       </c>
-      <c r="I33" s="4">
-        <v>25</v>
-      </c>
-      <c r="J33" s="4">
-        <v>99</v>
-      </c>
-      <c r="K33" s="4">
-        <v>25</v>
-      </c>
-      <c r="L33" s="4">
+      <c r="I33" s="3">
+        <v>25</v>
+      </c>
+      <c r="J33" s="3">
+        <v>99</v>
+      </c>
+      <c r="K33" s="3">
+        <v>25</v>
+      </c>
+      <c r="L33" s="3">
         <v>100</v>
       </c>
       <c r="M33" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>42</v>
+      <c r="A34" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B34" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZM-350_Marine-8</v>
+        <v>RZM-200-5</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
       </c>
       <c r="F34" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G34" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H34" s="2">
-        <v>1150</v>
+        <v>500</v>
       </c>
       <c r="I34" s="3">
         <v>25</v>
@@ -2051,174 +2039,90 @@
         <v>100</v>
       </c>
       <c r="M34" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>42</v>
+      <c r="A35" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B35" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZM-350_Marine-5</v>
+        <v>RZM-200-3</v>
       </c>
       <c r="E35" s="4">
         <v>1</v>
       </c>
-      <c r="F35" s="3">
-        <v>100</v>
-      </c>
-      <c r="G35" s="3">
-        <v>100</v>
-      </c>
-      <c r="H35" s="2">
-        <v>1150</v>
-      </c>
-      <c r="I35" s="3">
-        <v>25</v>
-      </c>
-      <c r="J35" s="3">
-        <v>99</v>
-      </c>
-      <c r="K35" s="3">
-        <v>25</v>
-      </c>
-      <c r="L35" s="3">
+      <c r="F35" s="4">
+        <v>20</v>
+      </c>
+      <c r="G35" s="4">
+        <v>20</v>
+      </c>
+      <c r="H35" s="4">
+        <v>500</v>
+      </c>
+      <c r="I35" s="4">
+        <v>25</v>
+      </c>
+      <c r="J35" s="4">
+        <v>99</v>
+      </c>
+      <c r="K35" s="4">
+        <v>25</v>
+      </c>
+      <c r="L35" s="4">
         <v>100</v>
       </c>
       <c r="M35" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B36" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RZM-200-5</v>
+        <v>RZM-200-2</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="4">
         <v>20</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="4">
         <v>20</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="4">
         <v>500</v>
       </c>
-      <c r="I36" s="3">
-        <v>25</v>
-      </c>
-      <c r="J36" s="3">
-        <v>99</v>
-      </c>
-      <c r="K36" s="3">
-        <v>25</v>
-      </c>
-      <c r="L36" s="3">
+      <c r="I36" s="4">
+        <v>25</v>
+      </c>
+      <c r="J36" s="4">
+        <v>99</v>
+      </c>
+      <c r="K36" s="4">
+        <v>25</v>
+      </c>
+      <c r="L36" s="4">
         <v>100</v>
       </c>
       <c r="M36" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="8">
-        <v>3</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>RZM-200-3</v>
-      </c>
-      <c r="E37" s="4">
-        <v>1</v>
-      </c>
-      <c r="F37" s="4">
-        <v>20</v>
-      </c>
-      <c r="G37" s="4">
-        <v>20</v>
-      </c>
-      <c r="H37" s="4">
-        <v>500</v>
-      </c>
-      <c r="I37" s="4">
-        <v>25</v>
-      </c>
-      <c r="J37" s="4">
-        <v>99</v>
-      </c>
-      <c r="K37" s="4">
-        <v>25</v>
-      </c>
-      <c r="L37" s="4">
-        <v>100</v>
-      </c>
-      <c r="M37" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="8">
-        <v>2</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>RZM-200-2</v>
-      </c>
-      <c r="E38" s="4">
-        <v>1</v>
-      </c>
-      <c r="F38" s="4">
-        <v>20</v>
-      </c>
-      <c r="G38" s="4">
-        <v>20</v>
-      </c>
-      <c r="H38" s="4">
-        <v>500</v>
-      </c>
-      <c r="I38" s="4">
-        <v>25</v>
-      </c>
-      <c r="J38" s="4">
-        <v>99</v>
-      </c>
-      <c r="K38" s="4">
-        <v>25</v>
-      </c>
-      <c r="L38" s="4">
-        <v>100</v>
-      </c>
-      <c r="M38" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>